<commit_message>
Committing the changes after implementing the extent reports
</commit_message>
<xml_diff>
--- a/KeywordFramework/src/test/java/dataEngine/DataEngine.xlsx
+++ b/KeywordFramework/src/test/java/dataEngine/DataEngine.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="82">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -275,6 +275,9 @@
   </si>
   <si>
     <t>Chrome</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -903,7 +906,7 @@
       </c>
       <c r="G10" s="4"/>
       <c r="H10" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1003,7 +1006,7 @@
       </c>
       <c r="G14" s="4"/>
       <c r="H14" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1220,7 +1223,7 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -1234,7 +1237,7 @@
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifed chrome driver path to execute in Azure DevOps
</commit_message>
<xml_diff>
--- a/KeywordFramework/src/test/java/dataEngine/DataEngine.xlsx
+++ b/KeywordFramework/src/test/java/dataEngine/DataEngine.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0190FB36-5AB2-4DDC-93F4-07542FFC47B1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C38FEF-2CE9-40C0-B393-A0619793FBA1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Steps" sheetId="1" r:id="rId1"/>
@@ -22,17 +22,23 @@
     <definedName name="Page_Name">Settings!$A$1:$A$13</definedName>
     <definedName name="Page_Name1">Settings!$A$2:$A$13</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="81">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -256,28 +262,25 @@
     <t>Validate that the saved contact is committed to data base</t>
   </si>
   <si>
+    <t>tbl_ContactSearch</t>
+  </si>
+  <si>
+    <t>Now check if the saved contact is in search results</t>
+  </si>
+  <si>
+    <t>findTextHTMLtable</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>tbl_ContactSearch</t>
-  </si>
-  <si>
-    <t>Now check if the saved contact is in search results</t>
-  </si>
-  <si>
-    <t>findTextHTMLtable</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Search</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -363,12 +366,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -653,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -711,10 +713,10 @@
         <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H2" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -736,7 +738,7 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -758,7 +760,7 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -784,7 +786,7 @@
         <v>41</v>
       </c>
       <c r="H5" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -810,7 +812,7 @@
         <v>38</v>
       </c>
       <c r="H6" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -834,7 +836,7 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -844,7 +846,7 @@
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -854,9 +856,9 @@
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="4"/>
       <c r="H8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -882,7 +884,7 @@
         <v>54</v>
       </c>
       <c r="H9" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -906,7 +908,7 @@
       </c>
       <c r="G10" s="4"/>
       <c r="H10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -929,10 +931,10 @@
         <v>29</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H11" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -955,10 +957,10 @@
         <v>29</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H12" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -982,7 +984,7 @@
       </c>
       <c r="G13" s="4"/>
       <c r="H13" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -1006,7 +1008,7 @@
       </c>
       <c r="G14" s="4"/>
       <c r="H14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1033,7 +1035,7 @@
         <v>Testing</v>
       </c>
       <c r="H15" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1057,10 +1059,10 @@
       </c>
       <c r="G16" s="4"/>
       <c r="H16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>69</v>
       </c>
@@ -1068,26 +1070,26 @@
         <v>53</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G17" s="4" t="str">
         <f>_xlfn.CONCAT(G11," ", G12)</f>
         <v>Testing Search</v>
       </c>
       <c r="H17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>69</v>
       </c>
@@ -1108,10 +1110,10 @@
       </c>
       <c r="G18" s="4"/>
       <c r="H18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>69</v>
       </c>
@@ -1129,10 +1131,10 @@
         <v>12</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H19" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1159,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73444656-1687-4992-B54B-834361992F29}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1195,7 +1197,7 @@
         <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1209,7 +1211,7 @@
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -1223,7 +1225,7 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -1237,7 +1239,7 @@
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1337,7 +1339,7 @@
         <v>63</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>24</v>
@@ -1422,7 +1424,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Commiting all changes related to TFS
</commit_message>
<xml_diff>
--- a/KeywordFramework/src/test/java/dataEngine/DataEngine.xlsx
+++ b/KeywordFramework/src/test/java/dataEngine/DataEngine.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C38FEF-2CE9-40C0-B393-A0619793FBA1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C990EF6-3468-4460-A70A-928FB8E30497}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Steps" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="93">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -271,16 +271,52 @@
     <t>findTextHTMLtable</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>Search</t>
-  </si>
-  <si>
     <t>Chrome</t>
   </si>
   <si>
+    <t>verifyElement</t>
+  </si>
+  <si>
+    <t>Genesis</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>chk_ContactSearch</t>
+  </si>
+  <si>
+    <t>Delete_Contact</t>
+  </si>
+  <si>
+    <t>voidAccept</t>
+  </si>
+  <si>
+    <t>CloseBrowser_1</t>
+  </si>
+  <si>
+    <t>Close Browser</t>
+  </si>
+  <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>Verify Username field</t>
+  </si>
+  <si>
+    <t>Verify Password Field</t>
+  </si>
+  <si>
+    <t>Verify login button</t>
+  </si>
+  <si>
+    <t>Check the checkbox</t>
+  </si>
+  <si>
+    <t>Click on delete button to delete contact</t>
+  </si>
+  <si>
+    <t>Click on Ok in windows pop-up</t>
   </si>
 </sst>
 </file>
@@ -653,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -713,10 +749,10 @@
         <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -738,7 +774,7 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -760,7 +796,7 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -771,7 +807,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>32</v>
@@ -780,13 +816,11 @@
         <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="G5" s="1"/>
       <c r="H5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -797,22 +831,22 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>38</v>
+      <c r="G6" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="H6" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -820,95 +854,97 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="H8" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>47</v>
+      <c r="C9" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>54</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="G9" s="3"/>
       <c r="H9" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>48</v>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -916,25 +952,21 @@
         <v>46</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>77</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G11" s="4"/>
       <c r="H11" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -942,25 +974,25 @@
         <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="H12" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -968,98 +1000,99 @@
         <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="H14" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="4" t="str">
-        <f>G11</f>
-        <v>Testing</v>
+      <c r="G15" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="H15" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -1067,26 +1100,23 @@
         <v>69</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="4" t="str">
-        <f>_xlfn.CONCAT(G11," ", G12)</f>
-        <v>Testing Search</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G17" s="4"/>
       <c r="H17" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -1094,23 +1124,26 @@
         <v>69</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="G18" s="4" t="str">
+        <f>G14</f>
+        <v>Genesis</v>
+      </c>
       <c r="H18" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -1118,39 +1151,184 @@
         <v>69</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="4" t="str">
+        <f>_xlfn.CONCAT(G14," ", G15)</f>
+        <v>Genesis Selenium</v>
+      </c>
+      <c r="H20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1" t="s">
+      <c r="E25" s="1"/>
+      <c r="F25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H19" t="s">
-        <v>80</v>
+      <c r="G25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D19" xr:uid="{2E21260B-0331-4EB3-89DC-22D8FAFE876C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D25" xr:uid="{2E21260B-0331-4EB3-89DC-22D8FAFE876C}">
       <formula1>Page_Name</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F19" xr:uid="{2B114343-A533-4C29-863F-CFFF1A9B7E35}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F25" xr:uid="{2B114343-A533-4C29-863F-CFFF1A9B7E35}">
       <formula1>Action_Keywords</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E19" xr:uid="{9BAFEE47-0498-43B3-A4BC-181D985CB3CA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E25" xr:uid="{9BAFEE47-0498-43B3-A4BC-181D985CB3CA}">
       <formula1>INDIRECT(D2)</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G6" r:id="rId1" display="Test@123" xr:uid="{EC58E303-D657-489B-BC90-11A0157A12CC}"/>
+    <hyperlink ref="G8" r:id="rId1" display="Test@123" xr:uid="{EC58E303-D657-489B-BC90-11A0157A12CC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1159,15 +1337,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73444656-1687-4992-B54B-834361992F29}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.1796875" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="49.08984375" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
   </cols>
@@ -1197,7 +1375,7 @@
         <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1211,35 +1389,49 @@
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1253,7 +1445,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1356,7 +1548,9 @@
         <v>44</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="F5" s="1" t="s">
         <v>29</v>
       </c>
@@ -1368,7 +1562,9 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="F6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1433,7 +1629,9 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
@@ -1441,7 +1639,9 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>